<commit_message>
Completed Individual Homework 3
</commit_message>
<xml_diff>
--- a/Week 3 - Resource Allocation/homework/Wk 3 HB WBS and Network Diagram labor estimate template.xlsx
+++ b/Week 3 - Resource Allocation/homework/Wk 3 HB WBS and Network Diagram labor estimate template.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My contents\au 2015 Online DL program revision materials\Case related materials\Building case materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksey\Desktop\PM420\Week 3\homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="9630" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
     <sheet name="Labor Resources" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="303">
   <si>
     <t>Task Name</t>
   </si>
@@ -939,7 +939,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -1199,6 +1199,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1234,6 +1251,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1388,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1441,7 +1475,7 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1460,7 +1494,7 @@
       <c r="F3" s="6">
         <v>4</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -1477,7 +1511,7 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -1498,7 +1532,9 @@
       <c r="F5" s="6">
         <v>5</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
@@ -1519,7 +1555,9 @@
       <c r="F6" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -1536,7 +1574,7 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -1557,7 +1595,9 @@
       <c r="F8" s="6">
         <v>14</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
@@ -1578,7 +1618,9 @@
       <c r="F9" s="6">
         <v>14</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
@@ -1599,7 +1641,9 @@
       <c r="F10" s="6">
         <v>14</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
@@ -1620,7 +1664,9 @@
       <c r="F11" s="6">
         <v>14</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
@@ -1641,7 +1687,9 @@
       <c r="F12" s="6">
         <v>14</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
@@ -1662,7 +1710,9 @@
       <c r="F13" s="6">
         <v>14</v>
       </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -1679,7 +1729,7 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
@@ -1700,7 +1750,9 @@
       <c r="F15" s="6">
         <v>15</v>
       </c>
-      <c r="G15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
@@ -1721,7 +1773,9 @@
       <c r="F16" s="6">
         <v>16</v>
       </c>
-      <c r="G16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
@@ -1742,7 +1796,9 @@
       <c r="F17" s="6">
         <v>18</v>
       </c>
-      <c r="G17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -1759,7 +1815,7 @@
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
@@ -1801,7 +1857,9 @@
       <c r="F20" s="6">
         <v>20</v>
       </c>
-      <c r="G20" s="4"/>
+      <c r="G20" s="4" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
@@ -1822,7 +1880,9 @@
       <c r="F21" s="6">
         <v>21</v>
       </c>
-      <c r="G21" s="4"/>
+      <c r="G21" s="4" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
@@ -1864,7 +1924,9 @@
       <c r="F23" s="6">
         <v>23</v>
       </c>
-      <c r="G23" s="4"/>
+      <c r="G23" s="4" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
@@ -1885,7 +1947,9 @@
       <c r="F24" s="6">
         <v>24</v>
       </c>
-      <c r="G24" s="4"/>
+      <c r="G24" s="4" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
@@ -1906,7 +1970,9 @@
       <c r="F25" s="6">
         <v>25</v>
       </c>
-      <c r="G25" s="4"/>
+      <c r="G25" s="4" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
@@ -1927,7 +1993,9 @@
       <c r="F26" s="6">
         <v>27</v>
       </c>
-      <c r="G26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -1944,7 +2012,7 @@
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
@@ -1965,7 +2033,9 @@
       <c r="F28" s="6">
         <v>28</v>
       </c>
-      <c r="G28" s="4"/>
+      <c r="G28" s="4" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
@@ -1986,7 +2056,9 @@
       <c r="F29" s="6">
         <v>29</v>
       </c>
-      <c r="G29" s="4"/>
+      <c r="G29" s="4" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
@@ -2007,7 +2079,9 @@
       <c r="F30" s="6">
         <v>30</v>
       </c>
-      <c r="G30" s="4"/>
+      <c r="G30" s="4" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
@@ -2028,7 +2102,9 @@
       <c r="F31" s="6">
         <v>31</v>
       </c>
-      <c r="G31" s="4"/>
+      <c r="G31" s="4" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
@@ -2049,7 +2125,9 @@
       <c r="F32" s="6">
         <v>32</v>
       </c>
-      <c r="G32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
@@ -2070,7 +2148,9 @@
       <c r="F33" s="6">
         <v>33</v>
       </c>
-      <c r="G33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
@@ -2091,7 +2171,9 @@
       <c r="F34" s="6">
         <v>34</v>
       </c>
-      <c r="G34" s="4"/>
+      <c r="G34" s="4" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
@@ -2112,7 +2194,9 @@
       <c r="F35" s="6">
         <v>35</v>
       </c>
-      <c r="G35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
@@ -2133,7 +2217,9 @@
       <c r="F36" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="G36" s="4"/>
+      <c r="G36" s="4" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
@@ -2154,7 +2240,9 @@
       <c r="F37" s="6">
         <v>38</v>
       </c>
-      <c r="G37" s="4"/>
+      <c r="G37" s="4" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
@@ -2171,7 +2259,7 @@
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
@@ -2192,7 +2280,9 @@
       <c r="F39" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="G39" s="4"/>
+      <c r="G39" s="4" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
@@ -2213,7 +2303,9 @@
       <c r="F40" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="G40" s="4"/>
+      <c r="G40" s="4" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
@@ -2234,7 +2326,9 @@
       <c r="F41" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="G41" s="4"/>
+      <c r="G41" s="4" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
@@ -2255,7 +2349,9 @@
       <c r="F42" s="6">
         <v>42</v>
       </c>
-      <c r="G42" s="4"/>
+      <c r="G42" s="4" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
@@ -2276,7 +2372,9 @@
       <c r="F43" s="6">
         <v>43</v>
       </c>
-      <c r="G43" s="4"/>
+      <c r="G43" s="4" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
@@ -2297,7 +2395,9 @@
       <c r="F44" s="6">
         <v>44</v>
       </c>
-      <c r="G44" s="4"/>
+      <c r="G44" s="4" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
@@ -2318,7 +2418,9 @@
       <c r="F45" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="G45" s="4"/>
+      <c r="G45" s="4" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
@@ -2335,7 +2437,7 @@
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
+      <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
@@ -2356,7 +2458,9 @@
       <c r="F47" s="6">
         <v>47</v>
       </c>
-      <c r="G47" s="4"/>
+      <c r="G47" s="4" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
@@ -2377,7 +2481,9 @@
       <c r="F48" s="6">
         <v>76</v>
       </c>
-      <c r="G48" s="4"/>
+      <c r="G48" s="4" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
@@ -2394,7 +2500,7 @@
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
+      <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
@@ -2415,7 +2521,9 @@
       <c r="F50" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="G50" s="4"/>
+      <c r="G50" s="4" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
@@ -2436,7 +2544,9 @@
       <c r="F51" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="G51" s="4"/>
+      <c r="G51" s="4" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
@@ -2457,7 +2567,9 @@
       <c r="F52" s="6">
         <v>107</v>
       </c>
-      <c r="G52" s="4"/>
+      <c r="G52" s="4" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
@@ -2478,7 +2590,9 @@
       <c r="F53" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="G53" s="4"/>
+      <c r="G53" s="4" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
@@ -2499,7 +2613,9 @@
       <c r="F54" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="G54" s="4"/>
+      <c r="G54" s="4" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
@@ -2520,7 +2636,9 @@
       <c r="F55" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="G55" s="4"/>
+      <c r="G55" s="4" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
@@ -2541,7 +2659,9 @@
       <c r="F56" s="6">
         <v>93</v>
       </c>
-      <c r="G56" s="4"/>
+      <c r="G56" s="4" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
@@ -2562,7 +2682,9 @@
       <c r="F57" s="6">
         <v>59</v>
       </c>
-      <c r="G57" s="4"/>
+      <c r="G57" s="4" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
@@ -2579,7 +2701,7 @@
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
+      <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
@@ -2596,7 +2718,7 @@
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
+      <c r="G59" s="1"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
@@ -2617,7 +2739,9 @@
       <c r="F60" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="G60" s="4"/>
+      <c r="G60" s="4" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
@@ -2638,7 +2762,9 @@
       <c r="F61" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="G61" s="4"/>
+      <c r="G61" s="4" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
@@ -2659,7 +2785,9 @@
       <c r="F62" s="6">
         <v>62</v>
       </c>
-      <c r="G62" s="4"/>
+      <c r="G62" s="4" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
@@ -2680,7 +2808,9 @@
       <c r="F63" s="6">
         <v>107</v>
       </c>
-      <c r="G63" s="4"/>
+      <c r="G63" s="4" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
@@ -2697,7 +2827,7 @@
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
+      <c r="G64" s="1"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
@@ -2718,7 +2848,9 @@
       <c r="F65" s="6">
         <v>65</v>
       </c>
-      <c r="G65" s="4"/>
+      <c r="G65" s="4" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
@@ -2739,7 +2871,9 @@
       <c r="F66" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="G66" s="4"/>
+      <c r="G66" s="4" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
@@ -2760,7 +2894,9 @@
       <c r="F67" s="6">
         <v>67</v>
       </c>
-      <c r="G67" s="4"/>
+      <c r="G67" s="4" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
@@ -2781,7 +2917,9 @@
       <c r="F68" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="G68" s="4"/>
+      <c r="G68" s="4" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
@@ -2802,7 +2940,9 @@
       <c r="F69" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="G69" s="4"/>
+      <c r="G69" s="4" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
@@ -2821,7 +2961,9 @@
         <v>263</v>
       </c>
       <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
+      <c r="G70" s="4" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
@@ -2838,7 +2980,7 @@
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
+      <c r="G71" s="1"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
@@ -2859,7 +3001,9 @@
       <c r="F72" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="G72" s="4"/>
+      <c r="G72" s="4" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
@@ -2880,7 +3024,9 @@
       <c r="F73" s="6">
         <v>73</v>
       </c>
-      <c r="G73" s="4"/>
+      <c r="G73" s="4" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
@@ -2901,7 +3047,9 @@
       <c r="F74" s="6">
         <v>78</v>
       </c>
-      <c r="G74" s="4"/>
+      <c r="G74" s="4" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
@@ -2922,7 +3070,9 @@
       <c r="F75" s="6">
         <v>75</v>
       </c>
-      <c r="G75" s="4"/>
+      <c r="G75" s="4" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
@@ -2941,7 +3091,9 @@
         <v>74</v>
       </c>
       <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
+      <c r="G76" s="4" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
@@ -2962,7 +3114,9 @@
       <c r="F77" s="6">
         <v>102</v>
       </c>
-      <c r="G77" s="4"/>
+      <c r="G77" s="4" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
@@ -2979,7 +3133,7 @@
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
+      <c r="G78" s="1"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
@@ -3000,7 +3154,9 @@
       <c r="F79" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="G79" s="4"/>
+      <c r="G79" s="4" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
@@ -3021,7 +3177,9 @@
       <c r="F80" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="G80" s="4"/>
+      <c r="G80" s="4" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
@@ -3042,7 +3200,9 @@
       <c r="F81" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="G81" s="4"/>
+      <c r="G81" s="4" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
@@ -3063,7 +3223,9 @@
       <c r="F82" s="6">
         <v>107</v>
       </c>
-      <c r="G82" s="4"/>
+      <c r="G82" s="4" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
@@ -3080,7 +3242,7 @@
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
-      <c r="G83" s="4"/>
+      <c r="G83" s="1"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
@@ -3101,7 +3263,9 @@
       <c r="F84" s="6">
         <v>84</v>
       </c>
-      <c r="G84" s="4"/>
+      <c r="G84" s="4" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
@@ -3122,7 +3286,9 @@
       <c r="F85" s="6">
         <v>85</v>
       </c>
-      <c r="G85" s="4"/>
+      <c r="G85" s="4" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
@@ -3143,7 +3309,9 @@
       <c r="F86" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="G86" s="4"/>
+      <c r="G86" s="4" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
@@ -3164,7 +3332,9 @@
       <c r="F87" s="7">
         <v>91107</v>
       </c>
-      <c r="G87" s="4"/>
+      <c r="G87" s="4" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
@@ -3181,7 +3351,7 @@
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
+      <c r="G88" s="1"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
@@ -3202,7 +3372,9 @@
       <c r="F89" s="6">
         <v>89</v>
       </c>
-      <c r="G89" s="4"/>
+      <c r="G89" s="4" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
@@ -3223,7 +3395,9 @@
       <c r="F90" s="6">
         <v>90</v>
       </c>
-      <c r="G90" s="4"/>
+      <c r="G90" s="4" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
@@ -3244,7 +3418,9 @@
       <c r="F91" s="7">
         <v>97107</v>
       </c>
-      <c r="G91" s="4"/>
+      <c r="G91" s="4" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
@@ -3265,7 +3441,9 @@
       <c r="F92" s="6">
         <v>93</v>
       </c>
-      <c r="G92" s="4"/>
+      <c r="G92" s="4" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
@@ -3282,7 +3460,7 @@
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
-      <c r="G93" s="4"/>
+      <c r="G93" s="1"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
@@ -3303,7 +3481,9 @@
       <c r="F94" s="6">
         <v>94</v>
       </c>
-      <c r="G94" s="4"/>
+      <c r="G94" s="4" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
@@ -3324,7 +3504,9 @@
       <c r="F95" s="6">
         <v>95</v>
       </c>
-      <c r="G95" s="4"/>
+      <c r="G95" s="4" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
@@ -3345,7 +3527,9 @@
       <c r="F96" s="7">
         <v>97107</v>
       </c>
-      <c r="G96" s="4"/>
+      <c r="G96" s="4" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
@@ -3362,7 +3546,7 @@
       </c>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
-      <c r="G97" s="4"/>
+      <c r="G97" s="1"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
@@ -3383,7 +3567,9 @@
       <c r="F98" s="6">
         <v>98</v>
       </c>
-      <c r="G98" s="4"/>
+      <c r="G98" s="4" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
@@ -3404,7 +3590,9 @@
       <c r="F99" s="6">
         <v>99</v>
       </c>
-      <c r="G99" s="4"/>
+      <c r="G99" s="4" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
@@ -3425,7 +3613,9 @@
       <c r="F100" s="6">
         <v>100</v>
       </c>
-      <c r="G100" s="4"/>
+      <c r="G100" s="4" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
@@ -3446,7 +3636,9 @@
       <c r="F101" s="7">
         <v>103108</v>
       </c>
-      <c r="G101" s="4"/>
+      <c r="G101" s="4" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
@@ -3463,7 +3655,7 @@
       </c>
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
-      <c r="G102" s="4"/>
+      <c r="G102" s="1"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
@@ -3484,7 +3676,9 @@
       <c r="F103" s="6">
         <v>103</v>
       </c>
-      <c r="G103" s="4"/>
+      <c r="G103" s="4" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
@@ -3505,7 +3699,9 @@
       <c r="F104" s="6">
         <v>104</v>
       </c>
-      <c r="G104" s="4"/>
+      <c r="G104" s="4" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
@@ -3526,7 +3722,9 @@
       <c r="F105" s="6">
         <v>105</v>
       </c>
-      <c r="G105" s="4"/>
+      <c r="G105" s="4" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
@@ -3547,7 +3745,9 @@
       <c r="F106" s="6">
         <v>107</v>
       </c>
-      <c r="G106" s="4"/>
+      <c r="G106" s="4" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
@@ -3564,7 +3764,7 @@
       </c>
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
-      <c r="G107" s="4"/>
+      <c r="G107" s="1"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
@@ -3585,7 +3785,9 @@
       <c r="F108" s="6">
         <v>108</v>
       </c>
-      <c r="G108" s="4"/>
+      <c r="G108" s="4" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
@@ -3606,7 +3808,9 @@
       <c r="F109" s="6">
         <v>109</v>
       </c>
-      <c r="G109" s="4"/>
+      <c r="G109" s="4" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
@@ -3627,7 +3831,9 @@
       <c r="F110" s="6">
         <v>110</v>
       </c>
-      <c r="G110" s="4"/>
+      <c r="G110" s="4" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
@@ -3648,7 +3854,9 @@
       <c r="F111" s="6">
         <v>111</v>
       </c>
-      <c r="G111" s="4"/>
+      <c r="G111" s="4" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
@@ -3667,11 +3875,23 @@
         <v>110</v>
       </c>
       <c r="F112" s="4"/>
-      <c r="G112" s="4"/>
+      <c r="G112" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Error Selecting Resource" error="Select resources from the list only.  Do not type anything in this cell.">
+          <x14:formula1>
+            <xm:f>'Labor Resources'!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>G5:G111</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3679,7 +3899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added week 4 homework - completed
</commit_message>
<xml_diff>
--- a/Week 3 - Resource Allocation/homework/Wk 3 HB WBS and Network Diagram labor estimate template.xlsx
+++ b/Week 3 - Resource Allocation/homework/Wk 3 HB WBS and Network Diagram labor estimate template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksey\Desktop\PM420\Week 3\homework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksey\Documents\School\UW_Project_Management\PROJECT_420\Week 3 - Resource Allocation\homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="304">
   <si>
     <t>Task Name</t>
   </si>
@@ -934,6 +934,9 @@
   </si>
   <si>
     <t>Estimated End</t>
+  </si>
+  <si>
+    <t>Days Only</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1105,7 +1108,15 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1420,24 +1431,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I106" sqref="I106"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="65" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="8" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="11" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" style="8" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1445,2437 +1458,2888 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="3">
+        <v>162</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2" s="4"/>
+      <c r="H2" s="1"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>238</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
+      <c r="C3" s="5">
+        <v>0</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="6">
+      <c r="E3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="6">
         <v>4</v>
       </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="3">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" s="4"/>
+      <c r="H4" s="1"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="5">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F5" s="6">
         <v>2</v>
       </c>
-      <c r="F5" s="6">
+      <c r="G5" s="6">
         <v>5</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
+      <c r="C6" s="5">
+        <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="6">
         <v>4</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="3">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" s="4"/>
+      <c r="H7" s="1"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="5">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="6">
+      <c r="F8" s="6">
         <v>5</v>
       </c>
-      <c r="F8" s="6">
+      <c r="G8" s="6">
         <v>14</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="5">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="6">
+      <c r="F9" s="6">
         <v>5</v>
       </c>
-      <c r="F9" s="6">
+      <c r="G9" s="6">
         <v>14</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="5">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="6">
+      <c r="F10" s="6">
         <v>5</v>
       </c>
-      <c r="F10" s="6">
+      <c r="G10" s="6">
         <v>14</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="5">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="6">
+      <c r="F11" s="6">
         <v>5</v>
       </c>
-      <c r="F11" s="6">
+      <c r="G11" s="6">
         <v>14</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="5">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="6">
+      <c r="F12" s="6">
         <v>5</v>
       </c>
-      <c r="F12" s="6">
+      <c r="G12" s="6">
         <v>14</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="5">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="6">
+      <c r="F13" s="6">
         <v>5</v>
       </c>
-      <c r="F13" s="6">
+      <c r="G13" s="6">
         <v>14</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14" s="4"/>
+      <c r="H14" s="1"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>30</v>
+      <c r="C15" s="5">
+        <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="F15" s="6">
+      <c r="G15" s="6">
         <v>15</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>34</v>
+      <c r="C16" s="5">
+        <v>1</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="6">
         <v>14</v>
       </c>
-      <c r="F16" s="6">
+      <c r="G16" s="6">
         <v>16</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>31</v>
+      <c r="C17" s="5">
+        <v>1</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="6">
         <v>15</v>
       </c>
-      <c r="F17" s="6">
+      <c r="G17" s="6">
         <v>18</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="3">
+        <v>42</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="4"/>
+      <c r="H18" s="1"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="5">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="6">
+      <c r="F19" s="6">
         <v>16</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="G19" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="4"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="5">
+        <v>13</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="6">
+      <c r="F20" s="6">
         <v>18</v>
       </c>
-      <c r="F20" s="6">
+      <c r="G20" s="6">
         <v>20</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="H20" s="4" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="5">
+        <v>12</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="6">
+      <c r="F21" s="6">
         <v>19</v>
       </c>
-      <c r="F21" s="6">
+      <c r="G21" s="6">
         <v>21</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="5">
+        <v>7</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="6">
+      <c r="F22" s="6">
         <v>20</v>
       </c>
-      <c r="F22" s="6">
+      <c r="G22" s="6">
         <v>22</v>
       </c>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="5">
+        <v>2</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="6">
+      <c r="F23" s="6">
         <v>21</v>
       </c>
-      <c r="F23" s="6">
+      <c r="G23" s="6">
         <v>23</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="5">
+        <v>2</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="6">
+      <c r="F24" s="6">
         <v>22</v>
       </c>
-      <c r="F24" s="6">
+      <c r="G24" s="6">
         <v>24</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>62</v>
+      <c r="C25" s="5">
+        <v>1</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="F25" s="6">
+      <c r="G25" s="6">
         <v>25</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="5">
+        <v>2</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="6">
+      <c r="F26" s="6">
         <v>24</v>
       </c>
-      <c r="F26" s="6">
+      <c r="G26" s="6">
         <v>27</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="3">
+        <v>22</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="4"/>
+      <c r="H27" s="1"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="5">
+        <v>2</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="6">
+      <c r="F28" s="6">
         <v>25</v>
       </c>
-      <c r="F28" s="6">
+      <c r="G28" s="6">
         <v>28</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="5">
+        <v>2</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="6">
+      <c r="F29" s="6">
         <v>27</v>
       </c>
-      <c r="F29" s="6">
+      <c r="G29" s="6">
         <v>29</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>74</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="5">
+        <v>4</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="6">
+      <c r="F30" s="6">
         <v>28</v>
       </c>
-      <c r="F30" s="6">
+      <c r="G30" s="6">
         <v>30</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="H30" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>78</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>79</v>
+      <c r="C31" s="5">
+        <v>1</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="6">
         <v>29</v>
       </c>
-      <c r="F31" s="6">
+      <c r="G31" s="6">
         <v>31</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="H31" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>80</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="5">
+        <v>2</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E32" s="6">
+      <c r="F32" s="6">
         <v>30</v>
       </c>
-      <c r="F32" s="6">
+      <c r="G32" s="6">
         <v>32</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>83</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="5">
+        <v>2</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="6">
+      <c r="F33" s="6">
         <v>31</v>
       </c>
-      <c r="F33" s="6">
+      <c r="G33" s="6">
         <v>33</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>86</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="5">
+        <v>3</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E34" s="6">
+      <c r="F34" s="6">
         <v>32</v>
       </c>
-      <c r="F34" s="6">
+      <c r="G34" s="6">
         <v>34</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="H34" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="5">
+        <v>2</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E35" s="6">
+      <c r="F35" s="6">
         <v>33</v>
       </c>
-      <c r="F35" s="6">
+      <c r="G35" s="6">
         <v>35</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="H35" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>92</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="5">
+        <v>3</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="6">
+      <c r="F36" s="6">
         <v>34</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="G36" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="H36" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>95</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>68</v>
+      <c r="C37" s="5">
+        <v>1</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="6">
         <v>35</v>
       </c>
-      <c r="F37" s="6">
+      <c r="G37" s="6">
         <v>38</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="H37" s="4" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="3">
+        <v>22</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G38" s="4"/>
+      <c r="H38" s="1"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>98</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="5">
+        <v>3</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="E39" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E39" s="6">
+      <c r="F39" s="6">
         <v>36</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="G39" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="H39" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="5">
+        <v>3</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E40" s="6">
+      <c r="F40" s="6">
         <v>38</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="H40" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>104</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="5">
+        <v>3</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="E41" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E41" s="6">
+      <c r="F41" s="6">
         <v>35</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="G41" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="H41" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="5">
+        <v>3</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="E42" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E42" s="6">
+      <c r="F42" s="6">
         <v>49</v>
       </c>
-      <c r="F42" s="6">
+      <c r="G42" s="6">
         <v>42</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="H42" s="4" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>109</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>110</v>
+      <c r="C43" s="5">
+        <v>1</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F43" s="6">
         <v>41</v>
       </c>
-      <c r="F43" s="6">
+      <c r="G43" s="6">
         <v>43</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="H43" s="4" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>111</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="5">
+        <v>3</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E44" s="6">
+      <c r="F44" s="6">
         <v>42</v>
       </c>
-      <c r="F44" s="6">
+      <c r="G44" s="6">
         <v>44</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="H44" s="4" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="5">
+        <v>3</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E45" s="6">
+      <c r="F45" s="6">
         <v>43</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="G45" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="H45" s="4" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="3">
+        <v>19</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G46" s="4"/>
+      <c r="H46" s="1"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>120</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="5">
+        <v>16</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="E47" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E47" s="6">
+      <c r="F47" s="6">
         <v>44</v>
       </c>
-      <c r="F47" s="6">
+      <c r="G47" s="6">
         <v>47</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="H47" s="4" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>123</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="5">
+        <v>3</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E48" s="6">
+      <c r="F48" s="6">
         <v>46</v>
       </c>
-      <c r="F48" s="6">
+      <c r="G48" s="6">
         <v>76</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="H48" s="4" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="3">
+        <v>21</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E49" s="4"/>
       <c r="F49" s="4"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G49" s="4"/>
+      <c r="H49" s="1"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>128</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="5">
+        <v>5</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="F50" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="G50" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="G50" s="4" t="s">
+      <c r="H50" s="4" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>132</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>107</v>
+      <c r="C51" s="5">
+        <v>1</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E51" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F51" s="6">
         <v>49</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="G51" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="H51" s="4" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>133</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="5">
+        <v>11</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="E52" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E52" s="6">
+      <c r="F52" s="6">
         <v>50</v>
       </c>
-      <c r="F52" s="6">
+      <c r="G52" s="6">
         <v>107</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="H52" s="4" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>136</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="5">
+        <v>5</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="E53" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="F53" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="G53" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="G53" s="4" t="s">
+      <c r="H53" s="4" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>137</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>107</v>
+      <c r="C54" s="5">
+        <v>1</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F54" s="6">
         <v>52</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="G54" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="H54" s="4" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>138</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="5">
+        <v>3</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="E55" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E55" s="6">
+      <c r="F55" s="6">
         <v>53</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="G55" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="H55" s="4" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>139</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>112</v>
+      <c r="C56" s="5">
+        <v>1</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E56" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F56" s="6">
         <v>54</v>
       </c>
-      <c r="F56" s="6">
+      <c r="G56" s="6">
         <v>93</v>
       </c>
-      <c r="G56" s="4" t="s">
+      <c r="H56" s="4" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>140</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="5">
+        <v>2</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="E57" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E57" s="6">
+      <c r="F57" s="6">
         <v>40</v>
       </c>
-      <c r="F57" s="6">
+      <c r="G57" s="6">
         <v>59</v>
       </c>
-      <c r="G57" s="4" t="s">
+      <c r="H57" s="4" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="3">
+        <v>30</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E58" s="4"/>
       <c r="F58" s="4"/>
-      <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G58" s="4"/>
+      <c r="H58" s="1"/>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="3">
+        <v>11</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="E59" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E59" s="4"/>
       <c r="F59" s="4"/>
-      <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G59" s="4"/>
+      <c r="H59" s="1"/>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>118</v>
+      <c r="C60" s="5">
+        <v>1</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="E60" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F60" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="F60" s="6" t="s">
+      <c r="G60" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="G60" s="4" t="s">
+      <c r="H60" s="4" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J60" s="5"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>127</v>
+      <c r="C61" s="5">
+        <v>1</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E61" s="6">
+      <c r="E61" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F61" s="6">
         <v>59</v>
       </c>
-      <c r="F61" s="6" t="s">
+      <c r="G61" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="G61" s="4" t="s">
+      <c r="H61" s="4" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>149</v>
+      <c r="C62" s="5">
+        <v>1</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E62" s="6" t="s">
+      <c r="E62" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F62" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="F62" s="6">
+      <c r="G62" s="6">
         <v>62</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="H62" s="4" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>150</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>145</v>
+      <c r="C63" s="5">
+        <v>1</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E63" s="6">
+      <c r="E63" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F63" s="6">
         <v>61</v>
       </c>
-      <c r="F63" s="6">
+      <c r="G63" s="6">
         <v>107</v>
       </c>
-      <c r="G63" s="4" t="s">
+      <c r="H63" s="4" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="3">
+        <v>9</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="E64" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E64" s="4"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G64" s="4"/>
+      <c r="H64" s="1"/>
+      <c r="J64" s="3"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>153</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="5">
+        <v>2</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="E65" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E65" s="6">
+      <c r="F65" s="6">
         <v>59</v>
       </c>
-      <c r="F65" s="6">
+      <c r="G65" s="6">
         <v>65</v>
       </c>
-      <c r="G65" s="4" t="s">
+      <c r="H65" s="4" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>155</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="5">
+        <v>2</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="E66" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E66" s="6">
+      <c r="F66" s="6">
         <v>64</v>
       </c>
-      <c r="F66" s="6" t="s">
+      <c r="G66" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="G66" s="4" t="s">
+      <c r="H66" s="4" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>158</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="5">
+        <v>2</v>
+      </c>
+      <c r="D67" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="E67" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E67" s="6" t="s">
+      <c r="F67" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="F67" s="6">
+      <c r="G67" s="6">
         <v>67</v>
       </c>
-      <c r="G67" s="4" t="s">
+      <c r="H67" s="4" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>161</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="5">
+        <v>2</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="E68" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E68" s="6">
+      <c r="F68" s="6">
         <v>66</v>
       </c>
-      <c r="F68" s="6" t="s">
+      <c r="G68" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="G68" s="4" t="s">
+      <c r="H68" s="4" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>164</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>159</v>
+      <c r="C69" s="5">
+        <v>1</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="E69" s="6">
+      <c r="E69" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F69" s="6">
         <v>65</v>
       </c>
-      <c r="F69" s="6" t="s">
+      <c r="G69" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="G69" s="4" t="s">
+      <c r="H69" s="4" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>165</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C70" s="5" t="s">
-        <v>149</v>
+      <c r="C70" s="5">
+        <v>1</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E70" s="6" t="s">
+      <c r="E70" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F70" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4" t="s">
+      <c r="G70" s="4"/>
+      <c r="H70" s="4" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>166</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" s="3">
+        <v>17</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="E71" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E71" s="4"/>
       <c r="F71" s="4"/>
-      <c r="G71" s="1"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G71" s="4"/>
+      <c r="H71" s="1"/>
+      <c r="J71" s="3"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>169</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C72" s="5" t="s">
-        <v>160</v>
+      <c r="C72" s="5">
+        <v>1</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E72" s="6">
+      <c r="E72" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F72" s="6">
         <v>68</v>
       </c>
-      <c r="F72" s="6" t="s">
+      <c r="G72" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="G72" s="4" t="s">
+      <c r="H72" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J72" s="5"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>170</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>162</v>
+      <c r="C73" s="5">
+        <v>1</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="E73" s="6">
+      <c r="E73" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F73" s="6">
         <v>71</v>
       </c>
-      <c r="F73" s="6">
+      <c r="G73" s="6">
         <v>73</v>
       </c>
-      <c r="G73" s="4" t="s">
+      <c r="H73" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J73" s="5"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>171</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C74" s="5" t="s">
-        <v>163</v>
+      <c r="C74" s="5">
+        <v>1</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E74" s="6">
+      <c r="E74" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F74" s="6">
         <v>72</v>
       </c>
-      <c r="F74" s="6">
+      <c r="G74" s="6">
         <v>78</v>
       </c>
-      <c r="G74" s="4" t="s">
+      <c r="H74" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
         <v>172</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C75" s="5" t="s">
-        <v>162</v>
+      <c r="C75" s="5">
+        <v>1</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="E75" s="6">
+      <c r="E75" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F75" s="6">
         <v>71</v>
       </c>
-      <c r="F75" s="6">
+      <c r="G75" s="6">
         <v>75</v>
       </c>
-      <c r="G75" s="4" t="s">
+      <c r="H75" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J75" s="5"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>173</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>163</v>
+      <c r="C76" s="5">
+        <v>1</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E76" s="6">
+      <c r="E76" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F76" s="6">
         <v>74</v>
       </c>
-      <c r="F76" s="4"/>
-      <c r="G76" s="4" t="s">
+      <c r="G76" s="4"/>
+      <c r="H76" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J76" s="5"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
         <v>174</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="5">
+        <v>4</v>
+      </c>
+      <c r="D77" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="E77" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="E77" s="6">
+      <c r="F77" s="6">
         <v>47</v>
       </c>
-      <c r="F77" s="6">
+      <c r="G77" s="6">
         <v>102</v>
       </c>
-      <c r="G77" s="4" t="s">
+      <c r="H77" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J77" s="5"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" s="3">
+        <v>6</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E78" s="4"/>
       <c r="F78" s="4"/>
-      <c r="G78" s="1"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G78" s="4"/>
+      <c r="H78" s="1"/>
+      <c r="J78" s="3"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>179</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="C79" s="5">
+        <v>2</v>
+      </c>
+      <c r="D79" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="E79" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E79" s="6">
+      <c r="F79" s="6">
         <v>73</v>
       </c>
-      <c r="F79" s="6" t="s">
+      <c r="G79" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="G79" s="4" t="s">
+      <c r="H79" s="4" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J79" s="5"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>180</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>181</v>
+      <c r="C80" s="5">
+        <v>1</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="E80" s="6">
+      <c r="E80" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F80" s="6">
         <v>78</v>
       </c>
-      <c r="F80" s="6" t="s">
+      <c r="G80" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="G80" s="4" t="s">
+      <c r="H80" s="4" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J80" s="5"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
         <v>182</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C81" s="5" t="s">
-        <v>183</v>
+      <c r="C81" s="5">
+        <v>1</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="E81" s="6">
+      <c r="E81" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F81" s="6">
         <v>79</v>
       </c>
-      <c r="F81" s="6" t="s">
+      <c r="G81" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="G81" s="4" t="s">
+      <c r="H81" s="4" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J81" s="5"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>184</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C82" s="5">
+        <v>2</v>
+      </c>
+      <c r="D82" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="E82" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E82" s="6">
+      <c r="F82" s="6">
         <v>80</v>
       </c>
-      <c r="F82" s="6">
+      <c r="G82" s="6">
         <v>107</v>
       </c>
-      <c r="G82" s="4" t="s">
+      <c r="H82" s="4" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J82" s="5"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C83" s="3">
+        <v>6</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="E83" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E83" s="4"/>
       <c r="F83" s="4"/>
-      <c r="G83" s="1"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G83" s="4"/>
+      <c r="H83" s="1"/>
+      <c r="J83" s="3"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>187</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C84" s="5" t="s">
-        <v>181</v>
+      <c r="C84" s="5">
+        <v>1</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="E84" s="6" t="s">
+      <c r="E84" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F84" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="F84" s="6">
+      <c r="G84" s="6">
         <v>84</v>
       </c>
-      <c r="G84" s="4" t="s">
+      <c r="H84" s="4" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J84" s="5"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>188</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C85" s="5">
+        <v>2</v>
+      </c>
+      <c r="D85" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="E85" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="E85" s="6" t="s">
+      <c r="F85" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="F85" s="6">
+      <c r="G85" s="6">
         <v>85</v>
       </c>
-      <c r="G85" s="4" t="s">
+      <c r="H85" s="4" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J85" s="5"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C86" s="5">
+        <v>2</v>
+      </c>
+      <c r="D86" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="E86" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E86" s="6" t="s">
+      <c r="F86" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="F86" s="6" t="s">
+      <c r="G86" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="G86" s="4" t="s">
+      <c r="H86" s="4" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J86" s="5"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>191</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C87" s="5" t="s">
-        <v>124</v>
+      <c r="C87" s="5">
+        <v>1</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E87" s="6">
+      <c r="E87" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F87" s="6">
         <v>85</v>
       </c>
-      <c r="F87" s="7">
+      <c r="G87" s="7">
         <v>91107</v>
       </c>
-      <c r="G87" s="4" t="s">
+      <c r="H87" s="4" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J87" s="5"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C88" s="3">
+        <v>3</v>
+      </c>
+      <c r="D88" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="E88" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E88" s="4"/>
       <c r="F88" s="4"/>
-      <c r="G88" s="1"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G88" s="4"/>
+      <c r="H88" s="1"/>
+      <c r="J88" s="3"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
         <v>193</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C89" s="5" t="s">
-        <v>124</v>
+      <c r="C89" s="5">
+        <v>1</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E89" s="6" t="s">
+      <c r="E89" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F89" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="F89" s="6">
+      <c r="G89" s="6">
         <v>89</v>
       </c>
-      <c r="G89" s="4" t="s">
+      <c r="H89" s="4" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J89" s="5"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
         <v>194</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C90" s="5" t="s">
-        <v>195</v>
+      <c r="C90" s="5">
+        <v>1</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="E90" s="6">
+      <c r="E90" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="F90" s="6">
         <v>88</v>
       </c>
-      <c r="F90" s="6">
+      <c r="G90" s="6">
         <v>90</v>
       </c>
-      <c r="G90" s="4" t="s">
+      <c r="H90" s="4" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J90" s="5"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
         <v>196</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C91" s="5" t="s">
-        <v>119</v>
+      <c r="C91" s="5">
+        <v>1</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E91" s="6">
+      <c r="E91" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F91" s="6">
         <v>89</v>
       </c>
-      <c r="F91" s="7">
+      <c r="G91" s="7">
         <v>97107</v>
       </c>
-      <c r="G91" s="4" t="s">
+      <c r="H91" s="4" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J91" s="5"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
         <v>197</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="C92" s="5">
+        <v>2</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="E92" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E92" s="6">
+      <c r="F92" s="6">
         <v>86</v>
       </c>
-      <c r="F92" s="6">
+      <c r="G92" s="6">
         <v>93</v>
       </c>
-      <c r="G92" s="4" t="s">
+      <c r="H92" s="4" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J92" s="5"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>198</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" s="3">
+        <v>3</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="E93" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E93" s="4"/>
       <c r="F93" s="4"/>
-      <c r="G93" s="1"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G93" s="4"/>
+      <c r="H93" s="1"/>
+      <c r="J93" s="3"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
         <v>200</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C94" s="5" t="s">
-        <v>175</v>
+      <c r="C94" s="5">
+        <v>1</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="E94" s="6" t="s">
+      <c r="E94" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F94" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="F94" s="6">
+      <c r="G94" s="6">
         <v>94</v>
       </c>
-      <c r="G94" s="4" t="s">
+      <c r="H94" s="4" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J94" s="5"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
         <v>201</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C95" s="5" t="s">
-        <v>202</v>
+      <c r="C95" s="5">
+        <v>1</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="E95" s="6">
+      <c r="E95" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F95" s="6">
         <v>93</v>
       </c>
-      <c r="F95" s="6">
+      <c r="G95" s="6">
         <v>95</v>
       </c>
-      <c r="G95" s="4" t="s">
+      <c r="H95" s="4" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J95" s="5"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
         <v>203</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C96" s="5" t="s">
-        <v>199</v>
+      <c r="C96" s="5">
+        <v>1</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="E96" s="6">
+      <c r="E96" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F96" s="6">
         <v>94</v>
       </c>
-      <c r="F96" s="7">
+      <c r="G96" s="7">
         <v>97107</v>
       </c>
-      <c r="G96" s="4" t="s">
+      <c r="H96" s="4" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J96" s="5"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C97" s="3">
+        <v>8</v>
+      </c>
+      <c r="D97" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="E97" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E97" s="4"/>
       <c r="F97" s="4"/>
-      <c r="G97" s="1"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G97" s="4"/>
+      <c r="H97" s="1"/>
+      <c r="J97" s="3"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
         <v>206</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="C98" s="5">
+        <v>3</v>
+      </c>
+      <c r="D98" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="E98" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="E98" s="6" t="s">
+      <c r="F98" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="F98" s="6">
+      <c r="G98" s="6">
         <v>98</v>
       </c>
-      <c r="G98" s="4" t="s">
+      <c r="H98" s="4" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J98" s="5"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
         <v>208</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C99" s="5" t="s">
+      <c r="C99" s="5">
+        <v>2</v>
+      </c>
+      <c r="D99" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="E99" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="E99" s="6">
+      <c r="F99" s="6">
         <v>97</v>
       </c>
-      <c r="F99" s="6">
+      <c r="G99" s="6">
         <v>99</v>
       </c>
-      <c r="G99" s="4" t="s">
+      <c r="H99" s="4" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J99" s="5"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
         <v>211</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C100" s="5">
+        <v>2</v>
+      </c>
+      <c r="D100" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="E100" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E100" s="6">
+      <c r="F100" s="6">
         <v>98</v>
       </c>
-      <c r="F100" s="6">
+      <c r="G100" s="6">
         <v>100</v>
       </c>
-      <c r="G100" s="4" t="s">
+      <c r="H100" s="4" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J100" s="5"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>214</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C101" s="5" t="s">
-        <v>143</v>
+      <c r="C101" s="5">
+        <v>1</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E101" s="6">
+      <c r="E101" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F101" s="6">
         <v>99</v>
       </c>
-      <c r="F101" s="7">
+      <c r="G101" s="7">
         <v>103108</v>
       </c>
-      <c r="G101" s="4" t="s">
+      <c r="H101" s="4" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J101" s="5"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>215</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="C102" s="3">
+        <v>12</v>
+      </c>
+      <c r="D102" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D102" s="3" t="s">
+      <c r="E102" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="E102" s="4"/>
       <c r="F102" s="4"/>
-      <c r="G102" s="1"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G102" s="4"/>
+      <c r="H102" s="1"/>
+      <c r="J102" s="3"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
         <v>218</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C103" s="5" t="s">
+      <c r="C103" s="5">
+        <v>2</v>
+      </c>
+      <c r="D103" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="E103" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="E103" s="6">
+      <c r="F103" s="6">
         <v>76</v>
       </c>
-      <c r="F103" s="6">
+      <c r="G103" s="6">
         <v>103</v>
       </c>
-      <c r="G103" s="4" t="s">
+      <c r="H103" s="4" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J103" s="5"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>219</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C104" s="5" t="s">
+      <c r="C104" s="5">
+        <v>2</v>
+      </c>
+      <c r="D104" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="D104" s="5" t="s">
+      <c r="E104" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="E104" s="7">
+      <c r="F104" s="7">
         <v>100102</v>
       </c>
-      <c r="F104" s="6">
+      <c r="G104" s="6">
         <v>104</v>
       </c>
-      <c r="G104" s="4" t="s">
+      <c r="H104" s="4" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J104" s="5"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
         <v>222</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C105" s="5" t="s">
+      <c r="C105" s="5">
+        <v>2</v>
+      </c>
+      <c r="D105" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D105" s="5" t="s">
+      <c r="E105" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="E105" s="6">
+      <c r="F105" s="6">
         <v>103</v>
       </c>
-      <c r="F105" s="6">
+      <c r="G105" s="6">
         <v>105</v>
       </c>
-      <c r="G105" s="4" t="s">
+      <c r="H105" s="4" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J105" s="5"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
         <v>225</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C106" s="5" t="s">
-        <v>217</v>
+      <c r="C106" s="5">
+        <v>1</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="E106" s="6">
+      <c r="E106" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F106" s="6">
         <v>104</v>
       </c>
-      <c r="F106" s="6">
+      <c r="G106" s="6">
         <v>107</v>
       </c>
-      <c r="G106" s="4" t="s">
+      <c r="H106" s="4" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J106" s="5"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>226</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C107" s="3">
+        <v>8</v>
+      </c>
+      <c r="D107" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="E107" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E107" s="4"/>
       <c r="F107" s="4"/>
-      <c r="G107" s="1"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G107" s="4"/>
+      <c r="H107" s="1"/>
+      <c r="J107" s="3"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
         <v>228</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C108" s="5" t="s">
-        <v>227</v>
+      <c r="C108" s="5">
+        <v>1</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="E108" s="6" t="s">
+      <c r="E108" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F108" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="F108" s="6">
+      <c r="G108" s="6">
         <v>108</v>
       </c>
-      <c r="G108" s="4" t="s">
+      <c r="H108" s="4" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J108" s="5"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
         <v>229</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C109" s="5" t="s">
-        <v>230</v>
+      <c r="C109" s="5">
+        <v>1</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="E109" s="7">
+      <c r="E109" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F109" s="7">
         <v>100107</v>
       </c>
-      <c r="F109" s="6">
+      <c r="G109" s="6">
         <v>109</v>
       </c>
-      <c r="G109" s="4" t="s">
+      <c r="H109" s="4" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J109" s="5"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
         <v>231</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C110" s="5" t="s">
-        <v>232</v>
+      <c r="C110" s="5">
+        <v>1</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="E110" s="6">
+      <c r="E110" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="F110" s="6">
         <v>108</v>
       </c>
-      <c r="F110" s="6">
+      <c r="G110" s="6">
         <v>110</v>
       </c>
-      <c r="G110" s="4" t="s">
+      <c r="H110" s="4" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J110" s="5"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
         <v>233</v>
       </c>
       <c r="B111" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C111" s="5" t="s">
+      <c r="C111" s="5">
+        <v>5</v>
+      </c>
+      <c r="D111" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="E111" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E111" s="6">
+      <c r="F111" s="6">
         <v>109</v>
       </c>
-      <c r="F111" s="6">
+      <c r="G111" s="6">
         <v>111</v>
       </c>
-      <c r="G111" s="4" t="s">
+      <c r="H111" s="4" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J111" s="5"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>273</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C112" s="5" t="s">
+      <c r="C112" s="5">
+        <v>0</v>
+      </c>
+      <c r="D112" s="15">
+        <v>41870</v>
+      </c>
+      <c r="E112" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D112" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E112" s="6">
+      <c r="F112" s="6">
         <v>110</v>
       </c>
-      <c r="F112" s="4"/>
-      <c r="G112" s="1"/>
+      <c r="G112" s="4"/>
+      <c r="H112" s="1"/>
+      <c r="J112" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3887,7 +4351,7 @@
           <x14:formula1>
             <xm:f>'Labor Resources'!$A$2:$A$25</xm:f>
           </x14:formula1>
-          <xm:sqref>G5:G111</xm:sqref>
+          <xm:sqref>H5:H111 H3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3899,16 +4363,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
@@ -3935,9 +4400,18 @@
       <c r="B2" s="13">
         <v>0</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="C2" s="16">
+        <f>SUMIF(WBS!H2:H112, "=" &amp; A2,WBS!C2:C112) * 8</f>
+        <v>8</v>
+      </c>
+      <c r="D2" s="17" t="str">
+        <f>WBS!D101</f>
+        <v>Thu 7/31/14</v>
+      </c>
+      <c r="E2" s="17" t="str">
+        <f>WBS!E101</f>
+        <v>Thu 7/31/14</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -3946,9 +4420,18 @@
       <c r="B3" s="13">
         <v>60</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="C3" s="16">
+        <f>SUMIF(WBS!H3:H113, "=" &amp; A3,WBS!C3:C113) * 8</f>
+        <v>160</v>
+      </c>
+      <c r="D3" s="17" t="str">
+        <f>WBS!D5</f>
+        <v>Mon 1/6/14</v>
+      </c>
+      <c r="E3" s="17" t="str">
+        <f>WBS!E5</f>
+        <v>Fri 1/31/14</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -3957,9 +4440,18 @@
       <c r="B4" s="13">
         <v>65</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
+      <c r="C4" s="16">
+        <f>SUMIF(WBS!H4:H114, "=" &amp; A4,WBS!C4:C114) * 8</f>
+        <v>272</v>
+      </c>
+      <c r="D4" s="17" t="str">
+        <f>WBS!D21</f>
+        <v>Mon 3/17/14</v>
+      </c>
+      <c r="E4" s="17" t="str">
+        <f>WBS!E23</f>
+        <v>Mon 4/14/14</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -3968,9 +4460,18 @@
       <c r="B5" s="13">
         <v>58</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+      <c r="C5" s="16">
+        <f>SUMIF(WBS!H5:H115, "=" &amp; A5,WBS!C5:C115) * 8</f>
+        <v>80</v>
+      </c>
+      <c r="D5" s="17" t="str">
+        <f>WBS!D65</f>
+        <v>Mon 6/23/14</v>
+      </c>
+      <c r="E5" s="17" t="str">
+        <f>WBS!E70</f>
+        <v>Thu 7/3/14</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -3979,9 +4480,18 @@
       <c r="B6" s="13">
         <v>0</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+      <c r="C6" s="16">
+        <f>SUMIF(WBS!H6:H116, "=" &amp; A6,WBS!C6:C116) * 8</f>
+        <v>16</v>
+      </c>
+      <c r="D6" s="17" t="str">
+        <f>WBS!D16</f>
+        <v>Wed 2/19/14</v>
+      </c>
+      <c r="E6" s="17" t="str">
+        <f>WBS!E16</f>
+        <v>Wed 2/19/14</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -3990,9 +4500,18 @@
       <c r="B7" s="13">
         <v>45</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
+      <c r="C7" s="16">
+        <f>SUMIF(WBS!H7:H117, "=" &amp; A7,WBS!C7:C117) * 8</f>
+        <v>80</v>
+      </c>
+      <c r="D7" s="17" t="str">
+        <f>WBS!D53</f>
+        <v>Fri 5/30/14</v>
+      </c>
+      <c r="E7" s="17" t="str">
+        <f>WBS!E53</f>
+        <v>Thu 6/5/14</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -4001,9 +4520,18 @@
       <c r="B8" s="13">
         <v>55</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
+      <c r="C8" s="16">
+        <f>SUMIF(WBS!H8:H118, "=" &amp; A8,WBS!C8:C118) * 8</f>
+        <v>16</v>
+      </c>
+      <c r="D8" s="17" t="str">
+        <f>WBS!D104</f>
+        <v>Fri 8/1/14</v>
+      </c>
+      <c r="E8" s="17" t="str">
+        <f>WBS!E104</f>
+        <v>Mon 8/4/14</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -4012,9 +4540,18 @@
       <c r="B9" s="13">
         <v>50</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+      <c r="C9" s="16">
+        <f>SUMIF(WBS!H9:H119, "=" &amp; A9,WBS!C9:C119) * 8</f>
+        <v>104</v>
+      </c>
+      <c r="D9" s="17" t="str">
+        <f>WBS!D43</f>
+        <v>Wed 6/11/14</v>
+      </c>
+      <c r="E9" s="17" t="str">
+        <f>WBS!E45</f>
+        <v>Thu 6/19/14</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -4023,9 +4560,18 @@
       <c r="B10" s="13">
         <v>76</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="C10" s="16">
+        <f>SUMIF(WBS!H10:H120, "=" &amp; A10,WBS!C10:C120) * 8</f>
+        <v>32</v>
+      </c>
+      <c r="D10" s="17" t="str">
+        <f>WBS!D99</f>
+        <v>Fri 7/25/14</v>
+      </c>
+      <c r="E10" s="17" t="str">
+        <f>WBS!E100</f>
+        <v>Wed 7/30/14</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -4034,9 +4580,18 @@
       <c r="B11" s="13">
         <v>40</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
+      <c r="C11" s="16">
+        <f>SUMIF(WBS!H11:H121, "=" &amp; A11,WBS!C11:C121) * 8</f>
+        <v>240</v>
+      </c>
+      <c r="D11" s="17" t="str">
+        <f>WBS!D28</f>
+        <v>Tue 4/22/14</v>
+      </c>
+      <c r="E11" s="17" t="str">
+        <f>WBS!E36</f>
+        <v>Tue 5/20/14</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
@@ -4045,9 +4600,18 @@
       <c r="B12" s="13">
         <v>70</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
+      <c r="C12" s="16">
+        <f>SUMIF(WBS!H12:H122, "=" &amp; A12,WBS!C12:C122) * 8</f>
+        <v>200</v>
+      </c>
+      <c r="D12" s="17" t="str">
+        <f>WBS!D3</f>
+        <v>Mon 1/6/14</v>
+      </c>
+      <c r="E12" s="17" t="str">
+        <f>WBS!E111</f>
+        <v>Tue 8/19/14</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
@@ -4056,9 +4620,18 @@
       <c r="B13" s="13">
         <v>80</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
+      <c r="C13" s="16">
+        <f>SUMIF(WBS!H13:H123, "=" &amp; A13,WBS!C13:C123) * 8</f>
+        <v>40</v>
+      </c>
+      <c r="D13" s="17" t="str">
+        <f>WBS!D55</f>
+        <v>Mon 6/9/14</v>
+      </c>
+      <c r="E13" s="17" t="str">
+        <f>WBS!E95</f>
+        <v>Fri 7/18/14</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -4067,9 +4640,18 @@
       <c r="B14" s="13">
         <v>0</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
+      <c r="C14" s="16">
+        <f>SUMIF(WBS!H14:H124, "=" &amp; A14,WBS!C14:C124) * 8</f>
+        <v>80</v>
+      </c>
+      <c r="D14" s="17" t="str">
+        <f>WBS!D25</f>
+        <v>Thu 4/17/14</v>
+      </c>
+      <c r="E14" s="17" t="str">
+        <f>WBS!E108</f>
+        <v>Fri 8/8/14</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -4078,9 +4660,18 @@
       <c r="B15" s="13">
         <v>90</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
+      <c r="C15" s="16">
+        <f>SUMIF(WBS!H15:H125, "=" &amp; A15,WBS!C15:C125) * 8</f>
+        <v>40</v>
+      </c>
+      <c r="D15" s="17" t="str">
+        <f>WBS!D24</f>
+        <v>Tue 4/15/14</v>
+      </c>
+      <c r="E15" s="17" t="str">
+        <f>WBS!E62</f>
+        <v>Thu 7/3/14</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
@@ -4089,9 +4680,18 @@
       <c r="B16" s="13">
         <v>40</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
+      <c r="C16" s="16">
+        <f>SUMIF(WBS!H16:H126, "=" &amp; A16,WBS!C16:C126) * 8</f>
+        <v>24</v>
+      </c>
+      <c r="D16" s="17" t="str">
+        <f>WBS!D105</f>
+        <v>Tue 8/5/14</v>
+      </c>
+      <c r="E16" s="17" t="str">
+        <f>WBS!E106</f>
+        <v>Thu 8/7/14</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
@@ -4100,9 +4700,18 @@
       <c r="B17" s="13">
         <v>50</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
+      <c r="C17" s="16">
+        <f>SUMIF(WBS!H17:H127, "=" &amp; A17,WBS!C17:C127) * 8</f>
+        <v>8</v>
+      </c>
+      <c r="D17" s="17" t="str">
+        <f>WBS!D109</f>
+        <v>Mon 8/11/14</v>
+      </c>
+      <c r="E17" s="17" t="str">
+        <f>WBS!E109</f>
+        <v>Mon 8/11/14</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
@@ -4111,9 +4720,18 @@
       <c r="B18" s="13">
         <v>80</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
+      <c r="C18" s="16">
+        <f>SUMIF(WBS!H18:H128, "=" &amp; A18,WBS!C18:C128) * 8</f>
+        <v>152</v>
+      </c>
+      <c r="D18" s="17" t="str">
+        <f>WBS!D47</f>
+        <v>Fri 6/20/14</v>
+      </c>
+      <c r="E18" s="17" t="str">
+        <f>WBS!E98</f>
+        <v>Thu 7/24/14</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
@@ -4122,9 +4740,18 @@
       <c r="B19" s="13">
         <v>0</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
+      <c r="C19" s="16">
+        <f>SUMIF(WBS!H19:H129, "=" &amp; A19,WBS!C19:C129) * 8</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="17" t="str">
+        <f>WBS!D6</f>
+        <v>Mon 2/3/14</v>
+      </c>
+      <c r="E19" s="17" t="str">
+        <f>WBS!E6</f>
+        <v>Mon 2/3/14</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
@@ -4133,9 +4760,18 @@
       <c r="B20" s="13">
         <v>0</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
+      <c r="C20" s="16">
+        <f>SUMIF(WBS!H20:H130, "=" &amp; A20,WBS!C20:C130) * 8</f>
+        <v>8</v>
+      </c>
+      <c r="D20" s="17" t="str">
+        <f>WBS!D110</f>
+        <v>Tue 8/12/14</v>
+      </c>
+      <c r="E20" s="17" t="str">
+        <f>WBS!E110</f>
+        <v>Tue 8/12/14</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
@@ -4144,9 +4780,18 @@
       <c r="B21" s="13">
         <v>47</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
+      <c r="C21" s="16">
+        <f>SUMIF(WBS!H21:H131, "=" &amp; A21,WBS!C21:C131) * 8</f>
+        <v>72</v>
+      </c>
+      <c r="D21" s="17" t="str">
+        <f>WBS!D72</f>
+        <v>Mon 6/30/14</v>
+      </c>
+      <c r="E21" s="17" t="str">
+        <f>WBS!E77</f>
+        <v>Tue 7/22/14</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -4155,9 +4800,18 @@
       <c r="B22" s="13">
         <v>45</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
+      <c r="C22" s="16">
+        <f>SUMIF(WBS!H22:H132, "=" &amp; A22,WBS!C22:C132) * 8</f>
+        <v>80</v>
+      </c>
+      <c r="D22" s="17" t="str">
+        <f>WBS!D50</f>
+        <v>Fri 5/30/14</v>
+      </c>
+      <c r="E22" s="17" t="str">
+        <f>WBS!E86</f>
+        <v>Fri 7/11/14</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
@@ -4166,9 +4820,18 @@
       <c r="B23" s="13">
         <v>50</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
+      <c r="C23" s="16">
+        <f>SUMIF(WBS!H23:H133, "=" &amp; A23,WBS!C23:C133) * 8</f>
+        <v>24</v>
+      </c>
+      <c r="D23" s="17" t="str">
+        <f>WBS!D42</f>
+        <v>Fri 6/6/14</v>
+      </c>
+      <c r="E23" s="17" t="str">
+        <f>WBS!E42</f>
+        <v>Tue 6/10/14</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
@@ -4177,9 +4840,18 @@
       <c r="B24" s="13">
         <v>42</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
+      <c r="C24" s="16">
+        <f>SUMIF(WBS!H24:H134, "=" &amp; A24,WBS!C24:C134) * 8</f>
+        <v>24</v>
+      </c>
+      <c r="D24" s="17" t="str">
+        <f>WBS!D48</f>
+        <v>Mon 7/14/14</v>
+      </c>
+      <c r="E24" s="17" t="str">
+        <f>WBS!E48</f>
+        <v>Wed 7/16/14</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
@@ -4188,9 +4860,18 @@
       <c r="B25" s="13">
         <v>150</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
+      <c r="C25" s="16">
+        <f>SUMIF(WBS!H25:H135, "=" &amp; A25,WBS!C25:C135) * 8</f>
+        <v>16</v>
+      </c>
+      <c r="D25" s="17" t="str">
+        <f>WBS!D15</f>
+        <v>Tue 2/18/14</v>
+      </c>
+      <c r="E25" s="17" t="str">
+        <f>WBS!E26</f>
+        <v>Mon 4/21/14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>